<commit_message>
initial commit prelim manuscript figure-making work
Primary plotting script is manuscript_figures.py. This script does almost only plotting stuff, so to-be-plotted data has to be selected and pickled during analysis in other scripts. This requires a few modifications and some hard coding.

The re-analyzed and exported data is saved into clockshift/analyzed_data.
</commit_message>
<xml_diff>
--- a/clockshift/dimer_metadata_file.xlsx
+++ b/clockshift/dimer_metadata_file.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\unobtainium\E_Carmen_Santiago\Analysis Scripts\analysis\clockshift\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\analysis\clockshift\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C164AC-7A58-4E3E-85FA-8FF209B2CF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="735" windowWidth="29400" windowHeight="16695"/>
+    <workbookView xWindow="-54720" yWindow="2415" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -197,7 +198,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -557,11 +558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>